<commit_message>
Atualizando importação das tabelas de docente. Correções do modelo de importação da tabela docentes_pesquisa.
</commit_message>
<xml_diff>
--- a/modelos/docente_pesquisa.xlsx
+++ b/modelos/docente_pesquisa.xlsx
@@ -41,12 +41,6 @@
     <t>Titulo do Projeto</t>
   </si>
   <si>
-    <t>Data de inicio do projeto de extensão</t>
-  </si>
-  <si>
-    <t>Data do fim do projeto de extensão</t>
-  </si>
-  <si>
     <t>Fonte</t>
   </si>
   <si>
@@ -54,6 +48,12 @@
   </si>
   <si>
     <t xml:space="preserve">Titulo do projeto de pesquisa do docente   </t>
+  </si>
+  <si>
+    <t>Data de inicio do projeto de pesquisa</t>
+  </si>
+  <si>
+    <t>Data do fim do projeto de pesquisa</t>
   </si>
 </sst>
 </file>
@@ -519,16 +519,16 @@
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="21.75" customHeight="1">
@@ -546,7 +546,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>4</v>
@@ -556,7 +556,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="26.25" customHeight="1">

</xml_diff>